<commit_message>
changed tables and sdsu
</commit_message>
<xml_diff>
--- a/data/closure_spreadsheet_final_2019.xlsx
+++ b/data/closure_spreadsheet_final_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/Fraternities and Sexual Assault/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/fraternities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56623D6E-799B-5A46-94D1-C31ED0E8F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDBA8F3-2986-B14E-ABAF-B28CB2DA1357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17800" windowHeight="21900" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30620" windowHeight="21900" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
   </bookViews>
   <sheets>
     <sheet name="closure_spreadsheet_main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="223">
   <si>
     <t>University</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>res_data_received</t>
+  </si>
+  <si>
+    <t>university enacted 3</t>
   </si>
 </sst>
 </file>
@@ -1208,21 +1211,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63494373-D1B0-2F4E-8589-31FBEC2D47DF}">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y38" sqref="Y38"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,64 +1250,67 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1318,43 +1326,44 @@
         <v>1</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
       <c r="K2" s="1"/>
-      <c r="N2" t="s">
+      <c r="L2" s="1"/>
+      <c r="O2" t="s">
         <v>66</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>128</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" s="22" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
         <v>162</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>200</v>
       </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1369,41 +1378,41 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>64</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
         <v>139</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" s="22" t="s">
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
         <v>163</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>201</v>
       </c>
-      <c r="Y3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1425,44 +1434,44 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>65</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>66</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
         <v>129</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" s="22" t="s">
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1477,29 +1486,29 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
         <v>59</v>
       </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1521,9 +1530,6 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="I6">
         <v>1</v>
       </c>
@@ -1531,40 +1537,43 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
         <v>66</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
         <v>128</v>
       </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6" s="22" t="s">
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6" t="s">
         <v>164</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>202</v>
       </c>
-      <c r="Y6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1579,35 +1588,35 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
         <v>63</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
         <v>88</v>
       </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7" s="22" t="s">
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="Y7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1622,35 +1631,35 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
         <v>66</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
         <v>130</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8" s="22" t="s">
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1663,32 +1672,32 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
         <v>66</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
         <v>128</v>
       </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9" s="22" t="s">
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1703,35 +1712,35 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
         <v>68</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>131</v>
       </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10" s="22" t="s">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1746,35 +1755,35 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
       <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
         <v>69</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
         <v>128</v>
       </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
-      <c r="U11" s="22" t="s">
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1789,35 +1798,35 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="N12" t="s">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
         <v>57</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
         <v>128</v>
       </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12" s="22" t="s">
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1832,41 +1841,41 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
       <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
         <v>70</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
         <v>128</v>
       </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13" s="22" t="s">
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="W13" t="s">
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13" t="s">
         <v>171</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>204</v>
       </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1888,47 +1897,47 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
-      <c r="N14" t="s">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
         <v>57</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>73</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
         <v>128</v>
       </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="U14" s="22" t="s">
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14" t="s">
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14" t="s">
         <v>172</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>205</v>
       </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1943,41 +1952,41 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="N15" t="s">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
         <v>71</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
         <v>128</v>
       </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15" s="22" t="s">
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" t="s">
         <v>173</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>206</v>
       </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1992,35 +2001,35 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="N16" t="s">
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
         <v>62</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
         <v>128</v>
       </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16" s="22" t="s">
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2035,38 +2044,38 @@
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
       <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
         <v>69</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
         <v>139</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17" s="22" t="s">
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="X17" t="s">
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="s">
         <v>218</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2081,35 +2090,35 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
       <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
         <v>66</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18" t="s">
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" t="s">
         <v>88</v>
       </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18" s="22" t="s">
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2124,35 +2133,35 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
       <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
         <v>66</v>
       </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19" t="s">
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
         <v>88</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19" s="22" t="s">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2167,41 +2176,41 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
       <c r="I20">
         <v>1</v>
       </c>
-      <c r="N20" t="s">
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="O20" t="s">
         <v>59</v>
       </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20" t="s">
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20" t="s">
         <v>128</v>
       </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
-      <c r="U20" s="22" t="s">
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" t="s">
         <v>178</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>208</v>
       </c>
-      <c r="Y20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -2214,38 +2223,38 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
         <v>59</v>
       </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21" t="s">
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21" t="s">
         <v>128</v>
       </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21" s="22" t="s">
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
-      <c r="W21" t="s">
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" t="s">
         <v>179</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>207</v>
       </c>
-      <c r="Y21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -2260,29 +2269,29 @@
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
       <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="N22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
         <v>57</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22" t="s">
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22" t="s">
         <v>128</v>
       </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2297,32 +2306,32 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
       <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="N23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
         <v>71</v>
       </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23" t="s">
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" t="s">
         <v>128</v>
       </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2337,94 +2346,100 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
       <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="N24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
         <v>68</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24" t="s">
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24" t="s">
         <v>132</v>
       </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-      <c r="U24" s="22" t="s">
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
+        <v>41968</v>
+      </c>
+      <c r="C25" s="3">
+        <v>42013</v>
+      </c>
+      <c r="D25" s="3">
         <v>43168</v>
       </c>
-      <c r="C25" s="3">
+      <c r="E25" s="3">
         <v>43377</v>
       </c>
-      <c r="D25" s="3">
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="M25" s="13">
         <v>43778</v>
       </c>
-      <c r="E25" s="3">
+      <c r="N25" s="13">
         <v>43847</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="14">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="L25" s="13">
-        <v>41968</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25" t="s">
         <v>71</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>57</v>
       </c>
-      <c r="P25" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25" t="s">
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25" t="s">
         <v>128</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
-      <c r="U25" s="22" t="s">
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="V25">
-        <v>0</v>
-      </c>
-      <c r="Y25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2434,35 +2449,37 @@
       <c r="C26" s="13">
         <v>43808</v>
       </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
         <v>56</v>
       </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26" t="s">
         <v>128</v>
       </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26" s="22" t="s">
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -2477,41 +2494,41 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="N27" t="s">
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
         <v>57</v>
       </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27" t="s">
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27" t="s">
         <v>88</v>
       </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="U27" s="22" t="s">
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27" t="s">
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27" t="s">
         <v>183</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>209</v>
       </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -2526,35 +2543,35 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="N28" t="s">
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
         <v>62</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28" t="s">
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" t="s">
         <v>133</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28" s="22" t="s">
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2567,32 +2584,32 @@
       <c r="F29">
         <v>1</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
         <v>57</v>
       </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29" t="s">
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29" t="s">
         <v>128</v>
       </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
-      <c r="U29" s="22" t="s">
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2607,32 +2624,32 @@
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
       <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="N30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
         <v>66</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30" t="s">
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30" t="s">
         <v>128</v>
       </c>
-      <c r="T30">
-        <v>1</v>
-      </c>
-      <c r="V30">
-        <v>0</v>
-      </c>
-      <c r="Y30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2647,9 +2664,6 @@
       <c r="F31" s="2">
         <v>0</v>
       </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
       <c r="I31">
         <v>1</v>
       </c>
@@ -2657,31 +2671,34 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="N31" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
         <v>59</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31" t="s">
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31" t="s">
         <v>128</v>
       </c>
-      <c r="T31">
-        <v>1</v>
-      </c>
-      <c r="U31" s="22" t="s">
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="Y31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2696,36 +2713,36 @@
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
       <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="N32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
         <v>69</v>
       </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32" t="s">
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32" t="s">
         <v>134</v>
       </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
-      <c r="U32" s="22"/>
-      <c r="V32">
-        <v>1</v>
-      </c>
-      <c r="X32" t="s">
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32" s="22"/>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="s">
         <v>203</v>
       </c>
-      <c r="Y32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2740,41 +2757,41 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
       <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="N33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
         <v>57</v>
       </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33" t="s">
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33" t="s">
         <v>139</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="U33" s="22" t="s">
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="V33">
-        <v>1</v>
-      </c>
-      <c r="W33" t="s">
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" t="s">
         <v>187</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>210</v>
       </c>
-      <c r="Y33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2789,41 +2806,41 @@
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="N34" t="s">
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
         <v>72</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34" t="s">
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34" t="s">
         <v>136</v>
       </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
-      <c r="U34" s="22" t="s">
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="V34">
-        <v>1</v>
-      </c>
-      <c r="W34" t="s">
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34" t="s">
         <v>188</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>211</v>
       </c>
-      <c r="Y34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -2838,38 +2855,38 @@
       <c r="F35">
         <v>0</v>
       </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="N35" t="s">
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
         <v>66</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35" t="s">
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35" t="s">
         <v>128</v>
       </c>
-      <c r="T35">
-        <v>1</v>
-      </c>
-      <c r="V35">
-        <v>1</v>
-      </c>
-      <c r="W35" t="s">
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35" t="s">
         <v>212</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>213</v>
       </c>
-      <c r="Y35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2884,41 +2901,41 @@
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="N36" t="s">
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
         <v>59</v>
       </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36" t="s">
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36" t="s">
         <v>128</v>
       </c>
-      <c r="T36">
-        <v>1</v>
-      </c>
-      <c r="U36" s="22" t="s">
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="V36">
-        <v>1</v>
-      </c>
-      <c r="W36" t="s">
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36" t="s">
         <v>189</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>214</v>
       </c>
-      <c r="Y36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -2933,35 +2950,35 @@
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
       <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="N37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
         <v>59</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37" t="s">
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37" t="s">
         <v>141</v>
       </c>
-      <c r="T37">
-        <v>1</v>
-      </c>
-      <c r="U37" s="22" t="s">
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="V37" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="V37">
-        <v>0</v>
-      </c>
-      <c r="Y37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -2976,41 +2993,41 @@
       <c r="F38">
         <v>1</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
       <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="N38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
         <v>68</v>
       </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38" t="s">
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38" t="s">
         <v>128</v>
       </c>
-      <c r="T38">
-        <v>1</v>
-      </c>
-      <c r="U38" s="22" t="s">
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="V38" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="V38">
-        <v>1</v>
-      </c>
-      <c r="W38" t="s">
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38" t="s">
         <v>191</v>
       </c>
-      <c r="X38" t="s">
+      <c r="Y38" t="s">
         <v>215</v>
       </c>
-      <c r="Y38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>84</v>
       </c>
@@ -3023,32 +3040,32 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
         <v>57</v>
       </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39" t="s">
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39" t="s">
         <v>128</v>
       </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39" s="22" t="s">
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="V39">
-        <v>1</v>
-      </c>
-      <c r="Y39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="Z39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -3061,32 +3078,32 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="O40" t="s">
         <v>57</v>
       </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40" t="s">
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40" t="s">
         <v>128</v>
       </c>
-      <c r="T40">
-        <v>1</v>
-      </c>
-      <c r="U40" s="22" t="s">
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="V40" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="V40">
-        <v>1</v>
-      </c>
-      <c r="Y40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -3101,41 +3118,41 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
       <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="N41" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
         <v>66</v>
       </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41" t="s">
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41" t="s">
         <v>128</v>
       </c>
-      <c r="T41">
-        <v>1</v>
-      </c>
-      <c r="U41" s="22" t="s">
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="V41" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="V41">
-        <v>1</v>
-      </c>
-      <c r="W41" t="s">
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41" t="s">
         <v>194</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>219</v>
       </c>
-      <c r="Y41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -3157,44 +3174,45 @@
       <c r="G42" s="14">
         <v>0</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
+      <c r="H42" s="14"/>
       <c r="I42">
         <v>1</v>
       </c>
-      <c r="N42" t="s">
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
         <v>73</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>57</v>
       </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42" t="s">
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42" t="s">
         <v>131</v>
       </c>
-      <c r="T42">
-        <v>1</v>
-      </c>
-      <c r="U42" s="22" t="s">
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="V42" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="V42">
-        <v>1</v>
-      </c>
-      <c r="W42" t="s">
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42" t="s">
         <v>195</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>216</v>
       </c>
-      <c r="Y42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="Z42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -3216,9 +3234,7 @@
       <c r="G43" s="1">
         <v>1</v>
       </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
+      <c r="H43" s="1"/>
       <c r="I43">
         <v>1</v>
       </c>
@@ -3226,194 +3242,197 @@
         <v>1</v>
       </c>
       <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="N43" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
         <v>57</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>56</v>
       </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43" t="s">
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43" t="s">
         <v>140</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>139</v>
       </c>
-      <c r="T43">
-        <v>1</v>
-      </c>
-      <c r="U43" s="22" t="s">
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="V43" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="V43">
-        <v>1</v>
-      </c>
-      <c r="W43" t="s">
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43" t="s">
         <v>196</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
         <v>217</v>
       </c>
-      <c r="Y43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>142</v>
       </c>
-      <c r="T44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="U44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="T45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="U45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>144</v>
       </c>
-      <c r="T46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="U46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>145</v>
       </c>
-      <c r="T47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="U47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>146</v>
       </c>
-      <c r="T48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="T49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="T50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="T51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>150</v>
       </c>
-      <c r="T52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="T53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="T54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="T55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="T56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="T57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="T58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="T59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="T60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="T61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="T62">
-        <f>SUM(T2:T61)</f>
+      <c r="U61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U62">
+        <f>SUM(U2:U61)</f>
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q43">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R43">
     <sortCondition ref="A11:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated hetero and results
</commit_message>
<xml_diff>
--- a/data/closure_spreadsheet_final_2019.xlsx
+++ b/data/closure_spreadsheet_final_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/fraternities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDBA8F3-2986-B14E-ABAF-B28CB2DA1357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14473F4-14DA-E246-9030-1867845A6347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30620" windowHeight="21900" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
+    <workbookView xWindow="38320" yWindow="500" windowWidth="30620" windowHeight="21100" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
   </bookViews>
   <sheets>
     <sheet name="closure_spreadsheet_main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="244">
   <si>
     <t>University</t>
   </si>
@@ -757,6 +757,69 @@
   </si>
   <si>
     <t>university enacted 3</t>
+  </si>
+  <si>
+    <t>Must have 100% of chapter go through a training session on social and risk reduction.</t>
+  </si>
+  <si>
+    <t>a series of intense educational programming sessions designed to make campus safer. Included alcohol skills training and sexual assault/bystander intervention traning.</t>
+  </si>
+  <si>
+    <t>guidelines_1</t>
+  </si>
+  <si>
+    <t>no third party vendors or anything, the students must "develop a plan to enhance education efforts and prgorams and create safer social environments when organizations host parties"</t>
+  </si>
+  <si>
+    <t>may regain privileges on oct 10 by "adhering to nationall recognized risk management policies and following certain guidelines for events involving alcohol"</t>
+  </si>
+  <si>
+    <t>guidelines_2</t>
+  </si>
+  <si>
+    <t>more training</t>
+  </si>
+  <si>
+    <t>lifted once divisoin of student affairs has conducted a review of the organization and each chempter's members have successfully completed additional education and training regarding alcohol, and high-risk behavior.</t>
+  </si>
+  <si>
+    <t>no information</t>
+  </si>
+  <si>
+    <t>"lift the ban once we have produced tangible and proactive steps mending the flaws in our social culture at Emory"</t>
+  </si>
+  <si>
+    <t>must complete "party 101 workshop offered by Owls Care Health Promotion"</t>
+  </si>
+  <si>
+    <t>"must complete risk management"</t>
+  </si>
+  <si>
+    <t>no more than 3 social events with alcohol per week and limited to 5 hours after</t>
+  </si>
+  <si>
+    <t>must complete training</t>
+  </si>
+  <si>
+    <t>"reviewed and strengthened campus policies"</t>
+  </si>
+  <si>
+    <t>greek leaders need to come up with a plan</t>
+  </si>
+  <si>
+    <t>"university committee will conduct a thorough investigation of current policies and procedures governing Greek activities"</t>
+  </si>
+  <si>
+    <t>"submit organizational plans"</t>
+  </si>
+  <si>
+    <t>not clear</t>
+  </si>
+  <si>
+    <t>"each fraternity participate in ongoing educational and leadership opportunities that promote responsibility and accountability"</t>
+  </si>
+  <si>
+    <t>training</t>
   </si>
 </sst>
 </file>
@@ -1211,11 +1274,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63494373-D1B0-2F4E-8589-31FBEC2D47DF}">
-  <dimension ref="A1:AA62"/>
+  <dimension ref="A1:AC62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G23" sqref="G23"/>
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1225,9 +1288,10 @@
     <col min="7" max="8" width="20.6640625" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
     <col min="22" max="22" width="14.33203125" customWidth="1"/>
+    <col min="28" max="28" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,8 +1373,14 @@
       <c r="AA1" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1362,8 +1432,11 @@
       <c r="Z2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1411,8 +1484,11 @@
       <c r="Z3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1470,8 +1546,14 @@
       <c r="Z4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1572,8 +1654,11 @@
       <c r="Z6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1615,8 +1700,11 @@
       <c r="Z7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1658,8 +1746,11 @@
       <c r="Z8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1696,8 +1787,11 @@
       <c r="Z9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1739,8 +1833,11 @@
       <c r="Z10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1782,8 +1879,11 @@
       <c r="Z11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1825,8 +1925,11 @@
       <c r="Z12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1874,8 +1977,11 @@
       <c r="Z13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1916,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="U14">
         <v>1</v>
@@ -1936,8 +2042,11 @@
       <c r="Z14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1986,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2028,8 +2137,11 @@
       <c r="Z16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2074,8 +2186,11 @@
       <c r="Z17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2103,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="U18">
         <v>1</v>
@@ -2118,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2161,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2209,8 +2324,11 @@
       <c r="Z20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -2253,8 +2371,11 @@
       <c r="Z21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -2291,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2330,8 +2451,11 @@
       <c r="Z23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2373,8 +2497,11 @@
       <c r="Z24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -2438,8 +2565,11 @@
       <c r="Z25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+      <c r="AB25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2479,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -2528,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -2571,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2609,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2649,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2698,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
update kevin march 9
</commit_message>
<xml_diff>
--- a/data/closure_spreadsheet_final_2019.xlsx
+++ b/data/closure_spreadsheet_final_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltopper/Desktop/fraternities/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A750C1B1-9084-034A-93C3-ABD3C8F8254B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010AD1CD-4EA0-8A49-8452-7CB136D337D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35900" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{DB1CA4CE-1639-914A-A925-15443BDD0288}"/>
   </bookViews>
   <sheets>
     <sheet name="closure_spreadsheet_main" sheetId="1" r:id="rId1"/>
@@ -1369,9 +1369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63494373-D1B0-2F4E-8589-31FBEC2D47DF}">
   <dimension ref="A1:AE62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC11" sqref="AC11"/>
+      <selection pane="topRight" activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2883,6 +2883,9 @@
       </c>
       <c r="AD27" t="s">
         <v>245</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="19" x14ac:dyDescent="0.25">

</xml_diff>